<commit_message>
Test uploadin img from excel
</commit_message>
<xml_diff>
--- a/excel_img.xlsx
+++ b/excel_img.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\cam-market-place\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developments\cam-market-place\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="3">
   <si>
     <t>Product Code</t>
   </si>
@@ -32,43 +32,13 @@
     <t>Picture</t>
   </si>
   <si>
-    <t>00078</t>
-  </si>
-  <si>
-    <t>O58756</t>
-  </si>
-  <si>
-    <t>O58758</t>
-  </si>
-  <si>
-    <t>O58759</t>
-  </si>
-  <si>
-    <t>O58760</t>
-  </si>
-  <si>
-    <t>O58761</t>
-  </si>
-  <si>
-    <t>O58762</t>
-  </si>
-  <si>
-    <t>O58763</t>
-  </si>
-  <si>
-    <t>O58764</t>
-  </si>
-  <si>
-    <t>O58765</t>
-  </si>
-  <si>
-    <t>O58766</t>
+    <t>P1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +106,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="O58271-1.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="O58271-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -174,7 +150,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="O58272-1.jpg"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="O58272-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,7 +194,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="O58273-1.jpg"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="O58273-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -250,7 +238,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="O58756-1.jpg"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="O58756-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -288,7 +282,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="O58757-1.jpg"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="O58757-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -326,7 +326,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="O58758-1.jpg"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="O58758-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -364,7 +370,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -402,7 +414,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -440,7 +458,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -478,7 +502,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -516,7 +546,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="14" name="Picture 13" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -554,7 +590,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="15" name="Picture 14" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -592,7 +634,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -630,7 +678,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="17" name="Picture 16" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -668,7 +722,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="18" name="Picture 17" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -706,7 +766,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="O58759-1.jpg"/>
+        <xdr:cNvPr id="19" name="Picture 18" descr="O58759-1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -997,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,62 +1098,62 @@
     </row>
     <row r="5" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>